<commit_message>
subject and year strength update
</commit_message>
<xml_diff>
--- a/26-10-2023_10-00 AM.xlsx
+++ b/26-10-2023_10-00 AM.xlsx
@@ -11,14 +11,13 @@
     <sheet name="G14" sheetId="2" r:id="rId2"/>
     <sheet name="G15" sheetId="3" r:id="rId3"/>
     <sheet name="S219" sheetId="4" r:id="rId4"/>
-    <sheet name="G13" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="9">
   <si>
     <t>Date = 26-10-2023</t>
   </si>
@@ -32,10 +31,10 @@
     <t>D2CSE_URN</t>
   </si>
   <si>
-    <t>D4CSE_CC</t>
+    <t>D3CSE_URN</t>
   </si>
   <si>
-    <t>D4CSE_NSC</t>
+    <t>D4CSE_DWDM</t>
   </si>
   <si>
     <t>G14</t>
@@ -45,9 +44,6 @@
   </si>
   <si>
     <t>S219</t>
-  </si>
-  <si>
-    <t>G13</t>
   </si>
 </sst>
 </file>
@@ -432,19 +428,19 @@
         <v>22000</v>
       </c>
       <c r="B5">
-        <v>2222000</v>
+        <v>21000</v>
       </c>
       <c r="C5">
-        <v>3333000</v>
+        <v>1111000</v>
       </c>
       <c r="D5">
         <v>22010</v>
       </c>
       <c r="E5">
-        <v>2222011</v>
+        <v>21011</v>
       </c>
       <c r="F5">
-        <v>3333009</v>
+        <v>1111009</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -452,19 +448,19 @@
         <v>22001</v>
       </c>
       <c r="B6">
-        <v>2222001</v>
+        <v>21001</v>
       </c>
       <c r="C6">
-        <v>3333001</v>
+        <v>1111001</v>
       </c>
       <c r="D6">
         <v>22011</v>
       </c>
       <c r="E6">
-        <v>2222012</v>
+        <v>21012</v>
       </c>
       <c r="F6">
-        <v>3333010</v>
+        <v>1111010</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -472,19 +468,19 @@
         <v>22002</v>
       </c>
       <c r="B7">
-        <v>2222002</v>
+        <v>21002</v>
       </c>
       <c r="C7">
-        <v>3333002</v>
+        <v>1111002</v>
       </c>
       <c r="D7">
         <v>22012</v>
       </c>
       <c r="E7">
-        <v>2222013</v>
+        <v>21013</v>
       </c>
       <c r="F7">
-        <v>3333011</v>
+        <v>1111011</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -492,19 +488,19 @@
         <v>22003</v>
       </c>
       <c r="B8">
-        <v>2222003</v>
+        <v>21003</v>
       </c>
       <c r="C8">
-        <v>3333003</v>
+        <v>1111003</v>
       </c>
       <c r="D8">
         <v>22013</v>
       </c>
       <c r="E8">
-        <v>2222014</v>
+        <v>21014</v>
       </c>
       <c r="F8">
-        <v>3333012</v>
+        <v>1111012</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -512,19 +508,19 @@
         <v>22004</v>
       </c>
       <c r="B9">
-        <v>2222004</v>
+        <v>21004</v>
       </c>
       <c r="C9">
-        <v>3333004</v>
+        <v>1111004</v>
       </c>
       <c r="D9">
         <v>22014</v>
       </c>
       <c r="E9">
-        <v>2222015</v>
+        <v>21015</v>
       </c>
       <c r="F9">
-        <v>3333013</v>
+        <v>1111013</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -532,19 +528,19 @@
         <v>22005</v>
       </c>
       <c r="B10">
-        <v>2222005</v>
+        <v>21005</v>
       </c>
       <c r="C10">
-        <v>3333005</v>
+        <v>1111005</v>
       </c>
       <c r="D10">
         <v>22015</v>
       </c>
       <c r="E10">
-        <v>2222016</v>
+        <v>21016</v>
       </c>
       <c r="F10">
-        <v>3333014</v>
+        <v>1111014</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -552,19 +548,19 @@
         <v>22006</v>
       </c>
       <c r="B11">
-        <v>2222006</v>
+        <v>21006</v>
       </c>
       <c r="C11">
-        <v>3333006</v>
+        <v>1111006</v>
       </c>
       <c r="D11">
         <v>22016</v>
       </c>
       <c r="E11">
-        <v>2222017</v>
+        <v>21017</v>
       </c>
       <c r="F11">
-        <v>3333015</v>
+        <v>1111015</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -572,19 +568,19 @@
         <v>22007</v>
       </c>
       <c r="B12">
-        <v>2222007</v>
+        <v>21007</v>
       </c>
       <c r="C12">
-        <v>3333007</v>
+        <v>1111007</v>
       </c>
       <c r="D12">
         <v>22017</v>
       </c>
       <c r="E12">
-        <v>2222018</v>
+        <v>21018</v>
       </c>
       <c r="F12">
-        <v>3333016</v>
+        <v>1111016</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -592,19 +588,19 @@
         <v>22008</v>
       </c>
       <c r="B13">
-        <v>2222008</v>
+        <v>21008</v>
       </c>
       <c r="C13">
-        <v>3333008</v>
+        <v>1111008</v>
       </c>
       <c r="D13">
         <v>22018</v>
       </c>
       <c r="E13">
-        <v>2222019</v>
+        <v>21019</v>
       </c>
       <c r="F13">
-        <v>3333017</v>
+        <v>1111017</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -612,12 +608,12 @@
         <v>22009</v>
       </c>
       <c r="B14">
-        <v>2222009</v>
+        <v>21009</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15">
-        <v>2222010</v>
+        <v>21010</v>
       </c>
     </row>
   </sheetData>
@@ -671,19 +667,19 @@
         <v>22019</v>
       </c>
       <c r="B5">
-        <v>2222020</v>
+        <v>21020</v>
       </c>
       <c r="C5">
-        <v>3333018</v>
+        <v>1111018</v>
       </c>
       <c r="D5">
         <v>22027</v>
       </c>
       <c r="E5">
-        <v>2222028</v>
+        <v>21028</v>
       </c>
       <c r="F5">
-        <v>3333026</v>
+        <v>1111026</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -691,19 +687,19 @@
         <v>22020</v>
       </c>
       <c r="B6">
-        <v>2222021</v>
+        <v>21021</v>
       </c>
       <c r="C6">
-        <v>3333019</v>
+        <v>1111019</v>
       </c>
       <c r="D6">
         <v>22028</v>
       </c>
       <c r="E6">
-        <v>2222029</v>
+        <v>21029</v>
       </c>
       <c r="F6">
-        <v>3333027</v>
+        <v>1111027</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -711,19 +707,19 @@
         <v>22021</v>
       </c>
       <c r="B7">
-        <v>2222022</v>
+        <v>21022</v>
       </c>
       <c r="C7">
-        <v>3333020</v>
+        <v>1111020</v>
       </c>
       <c r="D7">
         <v>22029</v>
       </c>
       <c r="E7">
-        <v>2222030</v>
+        <v>21030</v>
       </c>
       <c r="F7">
-        <v>3333028</v>
+        <v>1111028</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -731,19 +727,19 @@
         <v>22022</v>
       </c>
       <c r="B8">
-        <v>2222023</v>
+        <v>21023</v>
       </c>
       <c r="C8">
-        <v>3333021</v>
+        <v>1111021</v>
       </c>
       <c r="D8">
         <v>22030</v>
       </c>
       <c r="E8">
-        <v>2222031</v>
+        <v>21031</v>
       </c>
       <c r="F8">
-        <v>3333029</v>
+        <v>1111029</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -751,19 +747,19 @@
         <v>22023</v>
       </c>
       <c r="B9">
-        <v>2222024</v>
+        <v>21024</v>
       </c>
       <c r="C9">
-        <v>3333022</v>
+        <v>1111022</v>
       </c>
       <c r="D9">
         <v>22031</v>
       </c>
       <c r="E9">
-        <v>2222032</v>
+        <v>21032</v>
       </c>
       <c r="F9">
-        <v>3333030</v>
+        <v>1111030</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -771,19 +767,19 @@
         <v>22024</v>
       </c>
       <c r="B10">
-        <v>2222025</v>
+        <v>21025</v>
       </c>
       <c r="C10">
-        <v>3333023</v>
+        <v>1111023</v>
       </c>
       <c r="D10">
         <v>22032</v>
       </c>
       <c r="E10">
-        <v>2222033</v>
+        <v>21033</v>
       </c>
       <c r="F10">
-        <v>3333031</v>
+        <v>1111031</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -791,19 +787,19 @@
         <v>22025</v>
       </c>
       <c r="B11">
-        <v>2222026</v>
+        <v>21026</v>
       </c>
       <c r="C11">
-        <v>3333024</v>
+        <v>1111024</v>
       </c>
       <c r="D11">
         <v>22033</v>
       </c>
       <c r="E11">
-        <v>2222034</v>
+        <v>21034</v>
       </c>
       <c r="F11">
-        <v>3333032</v>
+        <v>1111032</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -811,19 +807,19 @@
         <v>22026</v>
       </c>
       <c r="B12">
-        <v>2222027</v>
+        <v>21027</v>
       </c>
       <c r="C12">
-        <v>3333025</v>
+        <v>1111025</v>
       </c>
       <c r="D12">
         <v>22034</v>
       </c>
       <c r="E12">
-        <v>2222035</v>
+        <v>21035</v>
       </c>
       <c r="F12">
-        <v>3333033</v>
+        <v>1111033</v>
       </c>
     </row>
   </sheetData>
@@ -877,19 +873,19 @@
         <v>22035</v>
       </c>
       <c r="B5">
-        <v>2222036</v>
+        <v>21036</v>
       </c>
       <c r="C5">
-        <v>3333034</v>
+        <v>1111034</v>
       </c>
       <c r="D5">
         <v>22042</v>
       </c>
       <c r="E5">
-        <v>2222043</v>
+        <v>21043</v>
       </c>
       <c r="F5">
-        <v>3333041</v>
+        <v>1111041</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -897,19 +893,19 @@
         <v>22036</v>
       </c>
       <c r="B6">
-        <v>2222037</v>
+        <v>21037</v>
       </c>
       <c r="C6">
-        <v>3333035</v>
+        <v>1111035</v>
       </c>
       <c r="D6">
         <v>22043</v>
       </c>
       <c r="E6">
-        <v>2222044</v>
+        <v>21044</v>
       </c>
       <c r="F6">
-        <v>3333042</v>
+        <v>1111042</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -917,19 +913,19 @@
         <v>22037</v>
       </c>
       <c r="B7">
-        <v>2222038</v>
+        <v>21038</v>
       </c>
       <c r="C7">
-        <v>3333036</v>
+        <v>1111036</v>
       </c>
       <c r="D7">
         <v>22044</v>
       </c>
       <c r="E7">
-        <v>2222045</v>
+        <v>21045</v>
       </c>
       <c r="F7">
-        <v>3333043</v>
+        <v>1111043</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -937,19 +933,19 @@
         <v>22038</v>
       </c>
       <c r="B8">
-        <v>2222039</v>
+        <v>21039</v>
       </c>
       <c r="C8">
-        <v>3333037</v>
+        <v>1111037</v>
       </c>
       <c r="D8">
         <v>22045</v>
       </c>
       <c r="E8">
-        <v>2222046</v>
+        <v>21046</v>
       </c>
       <c r="F8">
-        <v>3333044</v>
+        <v>1111044</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -957,19 +953,19 @@
         <v>22039</v>
       </c>
       <c r="B9">
-        <v>2222040</v>
+        <v>21040</v>
       </c>
       <c r="C9">
-        <v>3333038</v>
+        <v>1111038</v>
       </c>
       <c r="D9">
         <v>22046</v>
       </c>
       <c r="E9">
-        <v>2222047</v>
+        <v>21047</v>
       </c>
       <c r="F9">
-        <v>3333045</v>
+        <v>1111045</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -977,19 +973,19 @@
         <v>22040</v>
       </c>
       <c r="B10">
-        <v>2222041</v>
+        <v>21041</v>
       </c>
       <c r="C10">
-        <v>3333039</v>
+        <v>1111039</v>
       </c>
       <c r="D10">
         <v>22047</v>
       </c>
       <c r="E10">
-        <v>2222048</v>
+        <v>21048</v>
       </c>
       <c r="F10">
-        <v>3333046</v>
+        <v>1111046</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -997,29 +993,29 @@
         <v>22041</v>
       </c>
       <c r="B11">
-        <v>2222042</v>
+        <v>21042</v>
       </c>
       <c r="C11">
-        <v>3333040</v>
+        <v>1111040</v>
       </c>
       <c r="D11">
         <v>22048</v>
       </c>
       <c r="E11">
-        <v>2222049</v>
+        <v>21049</v>
       </c>
       <c r="F11">
-        <v>3333047</v>
+        <v>1111047</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="F12">
-        <v>3333048</v>
+        <v>1111048</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="F13">
-        <v>3333049</v>
+        <v>1111049</v>
       </c>
     </row>
   </sheetData>
@@ -1073,19 +1069,19 @@
         <v>22049</v>
       </c>
       <c r="B5">
-        <v>2222050</v>
+        <v>21050</v>
       </c>
       <c r="C5">
-        <v>3333050</v>
+        <v>1111050</v>
       </c>
       <c r="D5">
         <v>22054</v>
       </c>
       <c r="E5">
-        <v>2222055</v>
+        <v>21055</v>
       </c>
       <c r="F5">
-        <v>3333055</v>
+        <v>1111055</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1093,19 +1089,19 @@
         <v>22050</v>
       </c>
       <c r="B6">
-        <v>2222051</v>
+        <v>21051</v>
       </c>
       <c r="C6">
-        <v>3333051</v>
+        <v>1111051</v>
       </c>
       <c r="D6">
         <v>22055</v>
       </c>
       <c r="E6">
-        <v>2222056</v>
+        <v>21056</v>
       </c>
       <c r="F6">
-        <v>3333056</v>
+        <v>1111056</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1113,19 +1109,19 @@
         <v>22051</v>
       </c>
       <c r="B7">
-        <v>2222052</v>
+        <v>21052</v>
       </c>
       <c r="C7">
-        <v>3333052</v>
+        <v>1111052</v>
       </c>
       <c r="D7">
         <v>22056</v>
       </c>
       <c r="E7">
-        <v>2222057</v>
+        <v>21057</v>
       </c>
       <c r="F7">
-        <v>3333057</v>
+        <v>1111057</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1133,19 +1129,19 @@
         <v>22052</v>
       </c>
       <c r="B8">
-        <v>2222053</v>
+        <v>21053</v>
       </c>
       <c r="C8">
-        <v>3333053</v>
+        <v>1111053</v>
       </c>
       <c r="D8">
         <v>22057</v>
       </c>
       <c r="E8">
-        <v>2222058</v>
+        <v>21058</v>
       </c>
       <c r="F8">
-        <v>3333058</v>
+        <v>1111058</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1153,226 +1149,43 @@
         <v>22053</v>
       </c>
       <c r="B9">
-        <v>2222054</v>
+        <v>21054</v>
       </c>
       <c r="C9">
-        <v>3333054</v>
+        <v>1111054</v>
       </c>
       <c r="D9">
         <v>22058</v>
       </c>
       <c r="E9">
-        <v>2222059</v>
+        <v>21059</v>
       </c>
       <c r="F9">
-        <v>3333059</v>
+        <v>1111059</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="E10">
-        <v>2222060</v>
+        <v>21060</v>
       </c>
       <c r="F10">
-        <v>3333060</v>
+        <v>1111060</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="E11">
-        <v>2222061</v>
+        <v>21061</v>
       </c>
       <c r="F11">
-        <v>3333061</v>
+        <v>1111061</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="E12">
-        <v>2222062</v>
+        <v>21062</v>
       </c>
       <c r="F12">
-        <v>3333062</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6" ht="30" customHeight="1">
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>22059</v>
-      </c>
-      <c r="B5">
-        <v>2222063</v>
-      </c>
-      <c r="C5">
-        <v>3333063</v>
-      </c>
-      <c r="D5">
-        <v>22069</v>
-      </c>
-      <c r="F5">
-        <v>22078</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>22060</v>
-      </c>
-      <c r="B6">
-        <v>2222064</v>
-      </c>
-      <c r="C6">
-        <v>3333064</v>
-      </c>
-      <c r="D6">
-        <v>22070</v>
-      </c>
-      <c r="F6">
-        <v>22079</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>22061</v>
-      </c>
-      <c r="B7">
-        <v>2222065</v>
-      </c>
-      <c r="C7">
-        <v>3333065</v>
-      </c>
-      <c r="D7">
-        <v>22071</v>
-      </c>
-      <c r="F7">
-        <v>22080</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>22062</v>
-      </c>
-      <c r="B8">
-        <v>2222066</v>
-      </c>
-      <c r="C8">
-        <v>3333066</v>
-      </c>
-      <c r="D8">
-        <v>22072</v>
-      </c>
-      <c r="F8">
-        <v>22081</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
-        <v>22063</v>
-      </c>
-      <c r="B9">
-        <v>2222067</v>
-      </c>
-      <c r="C9">
-        <v>3333067</v>
-      </c>
-      <c r="D9">
-        <v>22073</v>
-      </c>
-      <c r="F9">
-        <v>22082</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
-        <v>22064</v>
-      </c>
-      <c r="B10">
-        <v>2222068</v>
-      </c>
-      <c r="C10">
-        <v>3333068</v>
-      </c>
-      <c r="D10">
-        <v>22074</v>
-      </c>
-      <c r="F10">
-        <v>22083</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
-        <v>22065</v>
-      </c>
-      <c r="D11">
-        <v>22075</v>
-      </c>
-      <c r="F11">
-        <v>22084</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
-        <v>22066</v>
-      </c>
-      <c r="D12">
-        <v>22076</v>
-      </c>
-      <c r="F12">
-        <v>22085</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13">
-        <v>22067</v>
-      </c>
-      <c r="D13">
-        <v>22077</v>
-      </c>
-      <c r="F13">
-        <v>22086</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14">
-        <v>22068</v>
+        <v>1111062</v>
       </c>
     </row>
   </sheetData>

</xml_diff>